<commit_message>
start and stop serializers
</commit_message>
<xml_diff>
--- a/src/data/staff_list.xlsx
+++ b/src/data/staff_list.xlsx
@@ -132,86 +132,86 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>22</v>
       </c>
     </row>

</xml_diff>